<commit_message>
Update von Recherche + Zeiterfassung
</commit_message>
<xml_diff>
--- a/Gesamt_Zeiterfassung_aktuell.xlsx
+++ b/Gesamt_Zeiterfassung_aktuell.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pargan\Documents\GitHub\IT_Projekt_SS19\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{623B99F3-6617-40DE-BABF-0605B24D9680}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E154E61C-5C03-4E2F-8A9F-35CE7118AFA3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1200" yWindow="468" windowWidth="20712" windowHeight="13272" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="29">
   <si>
     <t xml:space="preserve">Dusanic </t>
   </si>
@@ -123,6 +123,9 @@
   <si>
     <t>Merisa Pargan</t>
   </si>
+  <si>
+    <t xml:space="preserve">Recherche zu CRM und Event - Lösungen </t>
+  </si>
 </sst>
 </file>
 
@@ -202,12 +205,14 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1043,7 +1048,7 @@
                   <c:v>6.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.5</c:v>
+                  <c:v>9.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2230,7 +2235,7 @@
       </c>
       <c r="E4" s="1">
         <f>Pargan!F57</f>
-        <v>7.5</v>
+        <v>9.5</v>
       </c>
       <c r="G4" s="5"/>
       <c r="H4" s="38"/>
@@ -10012,8 +10017,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A2:F242"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10168,13 +10173,21 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B13" s="19"/>
-      <c r="C13" s="20"/>
-      <c r="D13" s="21"/>
-      <c r="E13" s="21"/>
+      <c r="B13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="20">
+        <v>43547</v>
+      </c>
+      <c r="D13" s="21">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="E13" s="21">
+        <v>0.6875</v>
+      </c>
       <c r="F13" s="24">
         <f>(Tabelle36[[#This Row],[bis]]*24)-(Tabelle36[[#This Row],[von]]*24)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -10616,7 +10629,7 @@
       <c r="E57" s="28"/>
       <c r="F57">
         <f>SUM(F8:F56)</f>
-        <v>7.5</v>
+        <v>9.5</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
update Zeiterfassung + Szenarien für Entscheidung
</commit_message>
<xml_diff>
--- a/Gesamt_Zeiterfassung_aktuell.xlsx
+++ b/Gesamt_Zeiterfassung_aktuell.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pargan\Documents\GitHub\IT_Projekt_SS19\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FA63B66-C938-4ED4-8024-B6678BB4688D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82CDE8AC-6E7E-40B6-91BF-3FC48E056408}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="624" yWindow="456" windowWidth="24960" windowHeight="14520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="67">
   <si>
     <t xml:space="preserve">Dusanic </t>
   </si>
@@ -236,6 +236,9 @@
   </si>
   <si>
     <t>Szenarien für Entscheidung schreiben weiter + weitere CRM Lösungen angeschaut/analysiert</t>
+  </si>
+  <si>
+    <t>Fertigstellung der Ebtscheidungsfindung</t>
   </si>
 </sst>
 </file>
@@ -1188,7 +1191,7 @@
                   <c:v>33.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40.5</c:v>
+                  <c:v>44.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2375,7 +2378,7 @@
       </c>
       <c r="E4" s="1">
         <f>Pargan!F55</f>
-        <v>40.5</v>
+        <v>44.5</v>
       </c>
       <c r="G4" s="5"/>
       <c r="H4" s="38"/>
@@ -2495,7 +2498,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:F245"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B21" sqref="B21:F21"/>
     </sheetView>
   </sheetViews>
@@ -10684,8 +10687,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A2:F242"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20:F20"/>
+    <sheetView topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11019,13 +11022,21 @@
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B23" s="23"/>
-      <c r="C23" s="20"/>
-      <c r="D23" s="21"/>
-      <c r="E23" s="21"/>
+      <c r="B23" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="C23" s="20">
+        <v>43591</v>
+      </c>
+      <c r="D23" s="21">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E23" s="21">
+        <v>0.58333333333333337</v>
+      </c>
       <c r="F23" s="24">
         <f>(Tabelle36[[#This Row],[bis]]*24)-(Tabelle36[[#This Row],[von]]*24)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.3">
@@ -11347,7 +11358,7 @@
       <c r="E55" s="28"/>
       <c r="F55">
         <f>SUM(F8:F54)</f>
-        <v>40.5</v>
+        <v>44.5</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>